<commit_message>
Update Gantt project planner.xlsx
</commit_message>
<xml_diff>
--- a/Design Phase/Gantt project planner.xlsx
+++ b/Design Phase/Gantt project planner.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28730"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E5C1224-F8E1-42F4-B2A0-4AFDF706AC11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{0E5C1224-F8E1-42F4-B2A0-4AFDF706AC11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8D0C5694-1278-47F2-B081-216E44D08556}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="58">
   <si>
     <t xml:space="preserve">Blackjack project Tasks </t>
   </si>
@@ -202,6 +202,12 @@
   </si>
   <si>
     <t>Implementation Phase</t>
+  </si>
+  <si>
+    <t>server (in the start) , player , penals and testing</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -1920,27 +1926,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22311CCC-0325-4A31-9EFD-58D1C23F0A25}">
   <dimension ref="A2:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="71" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="36.125" customWidth="1"/>
-    <col min="2" max="2" width="29.625" customWidth="1"/>
-    <col min="3" max="3" width="45.625" customWidth="1"/>
-    <col min="4" max="4" width="33.625" customWidth="1"/>
-    <col min="5" max="5" width="19.875" customWidth="1"/>
-    <col min="6" max="6" width="21.375" customWidth="1"/>
-    <col min="7" max="7" width="8.625" customWidth="1"/>
+    <col min="1" max="1" width="36.08203125" customWidth="1"/>
+    <col min="2" max="2" width="29.58203125" customWidth="1"/>
+    <col min="3" max="3" width="45.58203125" customWidth="1"/>
+    <col min="4" max="4" width="33.58203125" customWidth="1"/>
+    <col min="5" max="5" width="19.83203125" customWidth="1"/>
+    <col min="6" max="6" width="21.33203125" customWidth="1"/>
+    <col min="7" max="7" width="8.58203125" customWidth="1"/>
     <col min="8" max="10" width="9.5" customWidth="1"/>
-    <col min="11" max="11" width="9.625" customWidth="1"/>
+    <col min="11" max="11" width="9.58203125" customWidth="1"/>
     <col min="12" max="12" width="9.5" customWidth="1"/>
-    <col min="13" max="13" width="9.625" customWidth="1"/>
+    <col min="13" max="13" width="9.58203125" customWidth="1"/>
     <col min="14" max="14" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1960,7 +1966,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1980,7 +1986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2000,7 +2006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2020,7 +2026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -2036,7 +2042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -2052,7 +2058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -2066,46 +2072,46 @@
       <c r="E8" s="4"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B27" s="3"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>12</v>
       </c>
@@ -2119,7 +2125,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>16</v>
       </c>
@@ -2133,7 +2139,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>20</v>
       </c>
@@ -2147,7 +2153,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>24</v>
       </c>
@@ -2161,7 +2167,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>28</v>
       </c>
@@ -2175,7 +2181,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -2189,7 +2195,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -2203,7 +2209,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>37</v>
       </c>
@@ -2217,7 +2223,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -2231,7 +2237,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -2245,7 +2251,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -2259,7 +2265,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>36</v>
       </c>
@@ -2273,58 +2279,58 @@
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>55</v>
       </c>
       <c r="B40" s="1"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>55</v>
       </c>
       <c r="B41" s="1"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>55</v>
       </c>
       <c r="B42" s="1"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>55</v>
       </c>
       <c r="B43" s="1"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>55</v>
       </c>
       <c r="B44" s="1"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>55</v>
       </c>
       <c r="B45" s="1"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B46" s="1"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B47" s="1"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B48" s="1"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B49" s="1"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B50" s="1"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>35</v>
       </c>
@@ -2344,7 +2350,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>18</v>
       </c>
@@ -2354,8 +2360,11 @@
       <c r="C53" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D53" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>22</v>
       </c>
@@ -2365,8 +2374,11 @@
       <c r="C54" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D54" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>26</v>
       </c>
@@ -2377,7 +2389,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>30</v>
       </c>
@@ -2391,7 +2403,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>33</v>
       </c>

</xml_diff>